<commit_message>
Updated monograph + fixed minor mistakes on Fitness test classes
</commit_message>
<xml_diff>
--- a/Documentos Auxiliares/To-do_list.xlsx
+++ b/Documentos Auxiliares/To-do_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Terminar monografia</t>
   </si>
@@ -92,9 +92,6 @@
       </rPr>
       <t>Help</t>
     </r>
-  </si>
-  <si>
-    <t>Uso de popuplação passada na geração de nova chave</t>
   </si>
   <si>
     <r>
@@ -171,6 +168,18 @@
   </si>
   <si>
     <t>Revisar monografia</t>
+  </si>
+  <si>
+    <t>Uso de população passada na geração de nova chave</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>TERMINADO</t>
+  </si>
+  <si>
+    <t>QUASE TERMINADO</t>
   </si>
 </sst>
 </file>
@@ -268,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -276,11 +285,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -291,8 +306,8 @@
   <colors>
     <mruColors>
       <color rgb="FFCC9900"/>
+      <color rgb="FFFFCC00"/>
       <color rgb="FF008000"/>
-      <color rgb="FFFFCC00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -304,9 +319,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -344,7 +359,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -416,7 +431,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -590,124 +605,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.7109375" customWidth="1"/>
     <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>17</v>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>16</v>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="2" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
       <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>